<commit_message>
Cleaned up names and added includes
</commit_message>
<xml_diff>
--- a/root/TimeSheet.xlsx
+++ b/root/TimeSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e_yacoub\Documents\hotkeys\root\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e_yacoub\Documents\hotkeys\DeeHotKee\root\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="2880" yWindow="0" windowWidth="28800" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="DeeHotKeeTemplateSheet" sheetId="1" r:id="rId1"/>
@@ -162,12 +162,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -186,6 +180,12 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,18 +492,18 @@
       </c>
     </row>
     <row r="3" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -534,40 +534,40 @@
       <c r="J4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="L4"/>
     </row>
     <row r="5" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="15">
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13">
         <f>DSUM(B7:J50,9,B4:J5)</f>
         <v>0</v>
       </c>
       <c r="L5" s="3"/>
     </row>
     <row r="6" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="20"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="18"/>
       <c r="L6"/>
     </row>
     <row r="7" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -586,7 +586,7 @@
       <c r="F7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="19" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -602,24 +602,24 @@
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="11" t="str">
+      <c r="B8" s="20"/>
+      <c r="C8" s="9" t="str">
         <f t="shared" ref="C8" si="0">SUBSTITUTE(RIGHT(G8,12),empty_character,"")</f>
         <v/>
       </c>
-      <c r="D8" s="11" t="str">
+      <c r="D8" s="9" t="str">
         <f t="shared" ref="D8" si="1">SUBSTITUTE(RIGHT(LEFT(G8,33),9),empty_character,"")</f>
         <v/>
       </c>
-      <c r="E8" s="11" t="str">
+      <c r="E8" s="9" t="str">
         <f t="shared" ref="E8:E45" si="2">SUBSTITUTE(RIGHT(LEFT(G8,58),23),empty_character,"")</f>
         <v/>
       </c>
-      <c r="F8" s="11" t="str">
+      <c r="F8" s="9" t="str">
         <f t="shared" ref="F8:F47" si="3">SUBSTITUTE(LEFT(RIGHT(G8,82),67),empty_character,"")</f>
         <v/>
       </c>
-      <c r="G8" s="21"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="3" t="str">
         <f t="shared" ref="H8:H43" si="4">LEFT(RIGHT(LEFT(G8,25),15),8)</f>
         <v/>
@@ -632,27 +632,27 @@
         <f t="shared" ref="J8:J43" ca="1" si="6">IF(ISERR(24*(I8-H8)),IF(ISERR(24*(NOW()-(TODAY()+H8))),0,24*(NOW()-(TODAY()+H8))),24*(I8-H8))</f>
         <v>0</v>
       </c>
-      <c r="K8" s="23"/>
+      <c r="K8" s="21"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="11" t="str">
+      <c r="B9" s="20"/>
+      <c r="C9" s="9" t="str">
         <f t="shared" ref="C9:C30" si="7">SUBSTITUTE(RIGHT(G9,12),empty_character,"")</f>
         <v/>
       </c>
-      <c r="D9" s="11" t="str">
+      <c r="D9" s="9" t="str">
         <f t="shared" ref="D9:D30" si="8">SUBSTITUTE(RIGHT(LEFT(G9,33),9),empty_character,"")</f>
         <v/>
       </c>
-      <c r="E9" s="11" t="str">
+      <c r="E9" s="9" t="str">
         <f t="shared" ref="E9:E30" si="9">SUBSTITUTE(RIGHT(LEFT(G9,58),23),empty_character,"")</f>
         <v/>
       </c>
-      <c r="F9" s="11" t="str">
+      <c r="F9" s="9" t="str">
         <f t="shared" ref="F9:F30" si="10">SUBSTITUTE(LEFT(RIGHT(G9,82),67),empty_character,"")</f>
         <v/>
       </c>
-      <c r="G9" s="21"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -665,27 +665,27 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K9" s="23"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D10" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E10" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F10" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G10" s="21"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D10" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E10" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F10" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G10" s="19"/>
       <c r="H10" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -698,27 +698,27 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K10" s="23"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D11" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E11" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F11" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G11" s="21"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D11" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E11" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F11" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G11" s="19"/>
       <c r="H11" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -731,27 +731,27 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K11" s="23"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D12" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E12" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F12" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G12" s="21"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D12" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E12" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F12" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G12" s="19"/>
       <c r="H12" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -764,26 +764,26 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K12" s="23"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C13" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D13" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E13" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F13" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G13" s="21"/>
+      <c r="C13" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D13" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E13" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F13" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G13" s="19"/>
       <c r="H13" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -796,26 +796,26 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K13" s="23"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C14" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D14" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E14" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F14" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G14" s="21"/>
+      <c r="C14" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D14" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E14" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F14" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G14" s="19"/>
       <c r="H14" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -828,26 +828,26 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K14" s="23"/>
+      <c r="K14" s="21"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C15" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D15" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E15" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F15" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G15" s="21"/>
+      <c r="C15" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D15" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E15" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F15" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G15" s="19"/>
       <c r="H15" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -860,27 +860,27 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K15" s="23"/>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="22"/>
-      <c r="C16" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D16" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E16" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F16" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G16" s="21"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E16" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F16" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G16" s="19"/>
       <c r="H16" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -893,27 +893,27 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="K16" s="23"/>
+      <c r="K16" s="21"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-      <c r="C17" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D17" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E17" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F17" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G17" s="21"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D17" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E17" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F17" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G17" s="19"/>
       <c r="H17" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -928,24 +928,24 @@
       </c>
     </row>
     <row r="18" spans="2:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="22"/>
-      <c r="C18" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D18" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E18" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F18" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G18" s="21"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D18" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E18" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F18" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G18" s="19"/>
       <c r="H18" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -963,24 +963,24 @@
       <c r="M18" s="5"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="22"/>
-      <c r="C19" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D19" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E19" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F19" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G19" s="21"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D19" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E19" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F19" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G19" s="19"/>
       <c r="H19" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -995,24 +995,24 @@
       </c>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="22"/>
-      <c r="C20" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D20" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E20" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F20" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G20" s="21"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D20" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E20" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F20" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G20" s="19"/>
       <c r="H20" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1027,24 +1027,24 @@
       </c>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="22"/>
-      <c r="C21" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D21" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E21" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F21" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G21" s="21"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D21" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E21" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F21" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G21" s="19"/>
       <c r="H21" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1059,26 +1059,26 @@
       </c>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D22" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E22" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F22" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G22" s="21"/>
+      <c r="C22" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D22" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E22" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F22" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G22" s="19"/>
       <c r="H22" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1093,24 +1093,24 @@
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B23" s="22"/>
-      <c r="C23" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D23" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E23" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F23" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G23" s="21"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D23" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E23" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F23" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G23" s="19"/>
       <c r="H23" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1125,24 +1125,24 @@
       </c>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B24" s="22"/>
-      <c r="C24" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D24" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E24" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F24" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G24" s="21"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D24" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E24" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F24" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G24" s="19"/>
       <c r="H24" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1157,24 +1157,24 @@
       </c>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B25" s="22"/>
-      <c r="C25" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D25" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E25" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F25" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D25" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E25" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F25" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G25" s="19"/>
       <c r="H25" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1187,30 +1187,30 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="L25" s="24"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="25"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="20"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="23"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="22"/>
-      <c r="C26" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D26" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E26" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F26" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G26" s="21"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D26" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E26" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F26" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G26" s="19"/>
       <c r="H26" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1223,30 +1223,30 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="L26" s="24"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="25"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="23"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B27" s="22"/>
-      <c r="C27" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D27" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E27" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F27" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G27" s="21"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D27" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E27" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F27" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G27" s="19"/>
       <c r="H27" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1259,28 +1259,28 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="N27" s="24"/>
-      <c r="O27" s="25"/>
+      <c r="N27" s="22"/>
+      <c r="O27" s="23"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B28" s="22"/>
-      <c r="C28" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D28" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E28" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F28" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G28" s="21"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D28" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E28" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F28" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G28" s="19"/>
       <c r="H28" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1293,28 +1293,28 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="N28" s="24"/>
-      <c r="O28" s="25"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="23"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="22"/>
-      <c r="C29" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D29" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E29" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F29" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G29" s="21"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D29" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E29" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F29" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G29" s="19"/>
       <c r="H29" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1327,28 +1327,28 @@
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
       </c>
-      <c r="N29" s="24"/>
-      <c r="O29" s="25"/>
+      <c r="N29" s="22"/>
+      <c r="O29" s="23"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="D30" s="11" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="E30" s="11" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="F30" s="11" t="str">
-        <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="G30" s="21"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="9" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="D30" s="9" t="str">
+        <f t="shared" si="8"/>
+        <v/>
+      </c>
+      <c r="E30" s="9" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F30" s="9" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="G30" s="19"/>
       <c r="H30" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1363,24 +1363,24 @@
       </c>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="22"/>
-      <c r="C31" s="11" t="str">
+      <c r="B31" s="20"/>
+      <c r="C31" s="9" t="str">
         <f t="shared" ref="C31:C42" si="11">SUBSTITUTE(RIGHT(G31,12),empty_character,"")</f>
         <v/>
       </c>
-      <c r="D31" s="11" t="str">
+      <c r="D31" s="9" t="str">
         <f t="shared" ref="D31:D42" si="12">SUBSTITUTE(RIGHT(LEFT(G31,33),9),empty_character,"")</f>
         <v/>
       </c>
-      <c r="E31" s="11" t="str">
+      <c r="E31" s="9" t="str">
         <f t="shared" ref="E31:E42" si="13">SUBSTITUTE(RIGHT(LEFT(G31,58),23),empty_character,"")</f>
         <v/>
       </c>
-      <c r="F31" s="11" t="str">
+      <c r="F31" s="9" t="str">
         <f t="shared" ref="F31:F42" si="14">SUBSTITUTE(LEFT(RIGHT(G31,82),67),empty_character,"")</f>
         <v/>
       </c>
-      <c r="G31" s="21"/>
+      <c r="G31" s="19"/>
       <c r="H31" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1395,24 +1395,24 @@
       </c>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="22"/>
-      <c r="C32" s="11" t="str">
+      <c r="B32" s="20"/>
+      <c r="C32" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D32" s="11" t="str">
+      <c r="D32" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E32" s="11" t="str">
+      <c r="E32" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F32" s="11" t="str">
+      <c r="F32" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G32" s="21"/>
+      <c r="G32" s="19"/>
       <c r="H32" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1427,24 +1427,24 @@
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B33" s="22"/>
-      <c r="C33" s="11" t="str">
+      <c r="B33" s="20"/>
+      <c r="C33" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D33" s="11" t="str">
+      <c r="D33" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E33" s="11" t="str">
+      <c r="E33" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F33" s="11" t="str">
+      <c r="F33" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G33" s="21"/>
+      <c r="G33" s="19"/>
       <c r="H33" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1459,24 +1459,24 @@
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B34" s="22"/>
-      <c r="C34" s="11" t="str">
+      <c r="B34" s="20"/>
+      <c r="C34" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D34" s="11" t="str">
+      <c r="D34" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E34" s="11" t="str">
+      <c r="E34" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F34" s="11" t="str">
+      <c r="F34" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G34" s="21"/>
+      <c r="G34" s="19"/>
       <c r="H34" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1491,24 +1491,24 @@
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B35" s="22"/>
-      <c r="C35" s="11" t="str">
+      <c r="B35" s="20"/>
+      <c r="C35" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D35" s="11" t="str">
+      <c r="D35" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E35" s="11" t="str">
+      <c r="E35" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F35" s="11" t="str">
+      <c r="F35" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G35" s="21"/>
+      <c r="G35" s="19"/>
       <c r="H35" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1523,24 +1523,24 @@
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B36" s="22"/>
-      <c r="C36" s="11" t="str">
+      <c r="B36" s="20"/>
+      <c r="C36" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D36" s="11" t="str">
+      <c r="D36" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E36" s="11" t="str">
+      <c r="E36" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F36" s="11" t="str">
+      <c r="F36" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G36" s="21"/>
+      <c r="G36" s="19"/>
       <c r="H36" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1555,24 +1555,24 @@
       </c>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B37" s="22"/>
-      <c r="C37" s="11" t="str">
+      <c r="B37" s="20"/>
+      <c r="C37" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D37" s="11" t="str">
+      <c r="D37" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E37" s="11" t="str">
+      <c r="E37" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F37" s="11" t="str">
+      <c r="F37" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G37" s="21"/>
+      <c r="G37" s="19"/>
       <c r="H37" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1587,24 +1587,24 @@
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B38" s="22"/>
-      <c r="C38" s="11" t="str">
+      <c r="B38" s="20"/>
+      <c r="C38" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D38" s="11" t="str">
+      <c r="D38" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E38" s="11" t="str">
+      <c r="E38" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F38" s="11" t="str">
+      <c r="F38" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G38" s="21"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1619,24 +1619,24 @@
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="22"/>
-      <c r="C39" s="11" t="str">
+      <c r="B39" s="20"/>
+      <c r="C39" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D39" s="11" t="str">
+      <c r="D39" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E39" s="11" t="str">
+      <c r="E39" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F39" s="11" t="str">
+      <c r="F39" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G39" s="21"/>
+      <c r="G39" s="19"/>
       <c r="H39" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1651,24 +1651,24 @@
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="22"/>
-      <c r="C40" s="11" t="str">
+      <c r="B40" s="20"/>
+      <c r="C40" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D40" s="11" t="str">
+      <c r="D40" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E40" s="11" t="str">
+      <c r="E40" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F40" s="11" t="str">
+      <c r="F40" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G40" s="21"/>
+      <c r="G40" s="19"/>
       <c r="H40" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1683,24 +1683,24 @@
       </c>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="22"/>
-      <c r="C41" s="11" t="str">
+      <c r="B41" s="20"/>
+      <c r="C41" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D41" s="11" t="str">
+      <c r="D41" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E41" s="11" t="str">
+      <c r="E41" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F41" s="11" t="str">
+      <c r="F41" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G41" s="21"/>
+      <c r="G41" s="19"/>
       <c r="H41" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1715,24 +1715,24 @@
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B42" s="22"/>
-      <c r="C42" s="11" t="str">
+      <c r="B42" s="20"/>
+      <c r="C42" s="9" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="D42" s="11" t="str">
+      <c r="D42" s="9" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E42" s="11" t="str">
+      <c r="E42" s="9" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="F42" s="11" t="str">
+      <c r="F42" s="9" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="G42" s="21"/>
+      <c r="G42" s="19"/>
       <c r="H42" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1747,24 +1747,24 @@
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B43" s="22"/>
-      <c r="C43" s="11" t="str">
+      <c r="B43" s="20"/>
+      <c r="C43" s="9" t="str">
         <f t="shared" ref="C43" si="15">SUBSTITUTE(RIGHT(G43,12),empty_character,"")</f>
         <v/>
       </c>
-      <c r="D43" s="11" t="str">
+      <c r="D43" s="9" t="str">
         <f t="shared" ref="D43" si="16">SUBSTITUTE(RIGHT(LEFT(G43,33),9),empty_character,"")</f>
         <v/>
       </c>
-      <c r="E43" s="11" t="str">
+      <c r="E43" s="9" t="str">
         <f t="shared" ref="E43" si="17">SUBSTITUTE(RIGHT(LEFT(G43,58),23),empty_character,"")</f>
         <v/>
       </c>
-      <c r="F43" s="11" t="str">
+      <c r="F43" s="9" t="str">
         <f t="shared" ref="F43" si="18">SUBSTITUTE(LEFT(RIGHT(G43,82),67),empty_character,"")</f>
         <v/>
       </c>
-      <c r="G43" s="21"/>
+      <c r="G43" s="19"/>
       <c r="H43" s="3" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1779,85 +1779,85 @@
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D44" s="11" t="str">
+      <c r="D44" s="9" t="str">
         <f t="shared" ref="D44" si="19">SUBSTITUTE(RIGHT(LEFT(G44,33),9),empty_character,"")</f>
         <v/>
       </c>
-      <c r="E44" s="11" t="str">
+      <c r="E44" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F44" s="11" t="str">
+      <c r="F44" s="9" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D45" s="11" t="str">
+      <c r="D45" s="9" t="str">
         <f t="shared" ref="D45:D53" si="20">SUBSTITUTE(RIGHT(LEFT(G52,33),9),empty_character,"")</f>
         <v/>
       </c>
-      <c r="E45" s="11" t="str">
+      <c r="E45" s="9" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="F45" s="11" t="str">
+      <c r="F45" s="9" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D46" s="11" t="str">
+      <c r="D46" s="9" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="F46" s="11" t="str">
+      <c r="F46" s="9" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D47" s="11" t="str">
+      <c r="D47" s="9" t="str">
         <f>SUBSTITUTE(RIGHT(LEFT(G54,33),9),empty_character,"")</f>
         <v/>
       </c>
-      <c r="F47" s="11" t="str">
+      <c r="F47" s="9" t="str">
         <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="D48" s="11" t="str">
+      <c r="D48" s="9" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D49" s="11" t="str">
+      <c r="D49" s="9" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="50" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D50" s="11" t="str">
+      <c r="D50" s="9" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="51" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D51" s="11" t="str">
+      <c r="D51" s="9" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="52" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D52" s="11" t="str">
+      <c r="D52" s="9" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
     </row>
     <row r="53" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D53" s="11" t="str">
+      <c r="D53" s="9" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>

</xml_diff>